<commit_message>
Librerías y comienzo ONNX
</commit_message>
<xml_diff>
--- a/salidas/recomendados.xlsx
+++ b/salidas/recomendados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,381 +462,343 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>492</v>
+        <v>419</v>
       </c>
       <c r="B2" t="n">
-        <v>55247</v>
+        <v>904</v>
       </c>
       <c r="C2" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D2" t="n">
-        <v>4.586571382422027</v>
+        <v>4.40346779511421</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Into the Wild (2007)</t>
+          <t>Rear Window (1954)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>492</v>
+        <v>419</v>
       </c>
       <c r="B3" t="n">
-        <v>2324</v>
+        <v>1204</v>
       </c>
       <c r="C3" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D3" t="n">
-        <v>4.568586663936189</v>
+        <v>4.383534274137288</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Life Is Beautiful (La Vita è bella) (1997)</t>
+          <t>Lawrence of Arabia (1962)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>492</v>
+        <v>419</v>
       </c>
       <c r="B4" t="n">
-        <v>898</v>
+        <v>246</v>
       </c>
       <c r="C4" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D4" t="n">
-        <v>4.555526537998352</v>
+        <v>4.381324393346412</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Philadelphia Story, The (1940)</t>
+          <t>Hoop Dreams (1994)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>492</v>
+        <v>419</v>
       </c>
       <c r="B5" t="n">
-        <v>1680</v>
+        <v>7361</v>
       </c>
       <c r="C5" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D5" t="n">
-        <v>4.555355335811551</v>
+        <v>4.378079465621082</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sliding Doors (1998)</t>
+          <t>Eternal Sunshine of the Spotless Mind (2004)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>492</v>
+        <v>419</v>
       </c>
       <c r="B6" t="n">
-        <v>105504</v>
+        <v>2324</v>
       </c>
       <c r="C6" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D6" t="n">
-        <v>4.536787576076017</v>
+        <v>4.37424505401661</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Captain Phillips (2013)</t>
+          <t>Life Is Beautiful (La Vita è bella) (1997)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>469</v>
+        <v>256</v>
       </c>
       <c r="B7" t="n">
-        <v>2959</v>
+        <v>7371</v>
       </c>
       <c r="C7" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D7" t="n">
-        <v>4.634336954353524</v>
+        <v>4.519098607437904</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Fight Club (1999)</t>
+          <t>Dogville (2003)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>469</v>
+        <v>256</v>
       </c>
       <c r="B8" t="n">
-        <v>741</v>
+        <v>6016</v>
       </c>
       <c r="C8" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D8" t="n">
-        <v>4.566481339888441</v>
+        <v>4.505543143517541</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Ghost in the Shell (Kôkaku kidôtai) (1995)</t>
+          <t>City of God (Cidade de Deus) (2002)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>469</v>
+        <v>256</v>
       </c>
       <c r="B9" t="n">
-        <v>4973</v>
+        <v>2542</v>
       </c>
       <c r="C9" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D9" t="n">
-        <v>4.491077774048473</v>
+        <v>4.478808819824815</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Amelie (Fabuleux destin d'Amélie Poulain, Le) (2001)</t>
+          <t>Lock, Stock &amp; Two Smoking Barrels (1998)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>469</v>
+        <v>256</v>
       </c>
       <c r="B10" t="n">
-        <v>1041</v>
+        <v>1242</v>
       </c>
       <c r="C10" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D10" t="n">
-        <v>4.468655056683984</v>
+        <v>4.474695418345246</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Secrets &amp; Lies (1996)</t>
+          <t>Glory (1989)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>469</v>
+        <v>256</v>
       </c>
       <c r="B11" t="n">
-        <v>1249</v>
+        <v>48516</v>
       </c>
       <c r="C11" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D11" t="n">
-        <v>4.457306538071758</v>
+        <v>4.462593355387727</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Femme Nikita, La (Nikita) (1990)</t>
+          <t>Departed, The (2006)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>235</v>
+        <v>70</v>
       </c>
       <c r="B12" t="n">
-        <v>1204</v>
+        <v>898</v>
       </c>
       <c r="C12" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D12" t="n">
-        <v>4.446471317185627</v>
+        <v>4.653532122802486</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Lawrence of Arabia (1962)</t>
+          <t>Philadelphia Story, The (1940)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>235</v>
+        <v>70</v>
       </c>
       <c r="B13" t="n">
-        <v>50</v>
+        <v>750</v>
       </c>
       <c r="C13" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D13" t="n">
-        <v>4.441849524979956</v>
+        <v>4.649597859379635</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Usual Suspects, The (1995)</t>
+          <t>Dr. Strangelove or: How I Learned to Stop Worrying and Love the Bomb (1964)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>235</v>
+        <v>70</v>
       </c>
       <c r="B14" t="n">
-        <v>750</v>
+        <v>1136</v>
       </c>
       <c r="C14" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D14" t="n">
-        <v>4.440371228533754</v>
+        <v>4.634275890776808</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Dr. Strangelove or: How I Learned to Stop Worrying and Love the Bomb (1964)</t>
+          <t>Monty Python and the Holy Grail (1975)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>235</v>
+        <v>70</v>
       </c>
       <c r="B15" t="n">
-        <v>1208</v>
+        <v>2959</v>
       </c>
       <c r="C15" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D15" t="n">
-        <v>4.425886316023822</v>
+        <v>4.624144333833454</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Apocalypse Now (1979)</t>
+          <t>Fight Club (1999)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="B16" t="n">
-        <v>1197</v>
+        <v>318</v>
       </c>
       <c r="C16" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D16" t="n">
-        <v>3.881221809677639</v>
+        <v>4.562637723843174</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Princess Bride, The (1987)</t>
+          <t>Shawshank Redemption, The (1994)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="B17" t="n">
-        <v>1104</v>
+        <v>858</v>
       </c>
       <c r="C17" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D17" t="n">
-        <v>3.809048463062753</v>
+        <v>4.417489923360288</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Streetcar Named Desire, A (1951)</t>
+          <t>Godfather, The (1972)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>334</v>
+        <v>241</v>
       </c>
       <c r="B18" t="n">
-        <v>912</v>
+        <v>1104</v>
       </c>
       <c r="C18" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D18" t="n">
-        <v>3.76591383523425</v>
+        <v>4.20735890635388</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Casablanca (1942)</t>
+          <t>Streetcar Named Desire, A (1951)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>334</v>
+        <v>241</v>
       </c>
       <c r="B19" t="n">
-        <v>1248</v>
+        <v>1208</v>
       </c>
       <c r="C19" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D19" t="n">
-        <v>3.747158294041225</v>
+        <v>4.204941180277887</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Touch of Evil (1958)</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>108</v>
-      </c>
-      <c r="B20" t="n">
-        <v>318</v>
-      </c>
-      <c r="C20" t="n">
-        <v>3.579442714350294</v>
-      </c>
-      <c r="D20" t="n">
-        <v>4.819822135702879</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Shawshank Redemption, The (1994)</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>108</v>
-      </c>
-      <c r="B21" t="n">
-        <v>904</v>
-      </c>
-      <c r="C21" t="n">
-        <v>3.579442714350294</v>
-      </c>
-      <c r="D21" t="n">
-        <v>4.689284119284837</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Rear Window (1954)</t>
+          <t>Apocalypse Now (1979)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modelo llm y contenedor api
</commit_message>
<xml_diff>
--- a/salidas/recomendados.xlsx
+++ b/salidas/recomendados.xlsx
@@ -462,235 +462,235 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>492</v>
+        <v>551</v>
       </c>
       <c r="B2" t="n">
-        <v>55247</v>
+        <v>527</v>
       </c>
       <c r="C2" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D2" t="n">
-        <v>4.586571382422027</v>
+        <v>4.186775383307318</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Into the Wild (2007)</t>
+          <t>Schindler's List (1993)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>492</v>
+        <v>551</v>
       </c>
       <c r="B3" t="n">
-        <v>2324</v>
+        <v>4995</v>
       </c>
       <c r="C3" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D3" t="n">
-        <v>4.568586663936189</v>
+        <v>4.164571353122853</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Life Is Beautiful (La Vita è bella) (1997)</t>
+          <t>Beautiful Mind, A (2001)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>492</v>
+        <v>551</v>
       </c>
       <c r="B4" t="n">
-        <v>898</v>
+        <v>1237</v>
       </c>
       <c r="C4" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D4" t="n">
-        <v>4.555526537998352</v>
+        <v>4.161605006459395</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Philadelphia Story, The (1940)</t>
+          <t>Seventh Seal, The (Sjunde inseglet, Det) (1957)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>492</v>
+        <v>551</v>
       </c>
       <c r="B5" t="n">
-        <v>1680</v>
+        <v>908</v>
       </c>
       <c r="C5" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D5" t="n">
-        <v>4.555355335811551</v>
+        <v>4.153959304081716</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sliding Doors (1998)</t>
+          <t>North by Northwest (1959)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>492</v>
+        <v>551</v>
       </c>
       <c r="B6" t="n">
-        <v>105504</v>
+        <v>74458</v>
       </c>
       <c r="C6" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D6" t="n">
-        <v>4.536787576076017</v>
+        <v>4.130819113350436</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Captain Phillips (2013)</t>
+          <t>Shutter Island (2010)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>469</v>
+        <v>376</v>
       </c>
       <c r="B7" t="n">
-        <v>2959</v>
+        <v>904</v>
       </c>
       <c r="C7" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D7" t="n">
-        <v>4.634336954353524</v>
+        <v>4.656571391246109</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Fight Club (1999)</t>
+          <t>Rear Window (1954)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>469</v>
+        <v>376</v>
       </c>
       <c r="B8" t="n">
-        <v>741</v>
+        <v>44555</v>
       </c>
       <c r="C8" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D8" t="n">
-        <v>4.566481339888441</v>
+        <v>4.624277208509492</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Ghost in the Shell (Kôkaku kidôtai) (1995)</t>
+          <t>Lives of Others, The (Das leben der Anderen) (2006)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>469</v>
+        <v>376</v>
       </c>
       <c r="B9" t="n">
-        <v>4973</v>
+        <v>50</v>
       </c>
       <c r="C9" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D9" t="n">
-        <v>4.491077774048473</v>
+        <v>4.526885072934204</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Amelie (Fabuleux destin d'Amélie Poulain, Le) (2001)</t>
+          <t>Usual Suspects, The (1995)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>469</v>
+        <v>376</v>
       </c>
       <c r="B10" t="n">
-        <v>1041</v>
+        <v>898</v>
       </c>
       <c r="C10" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D10" t="n">
-        <v>4.468655056683984</v>
+        <v>4.526047604530664</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Secrets &amp; Lies (1996)</t>
+          <t>Philadelphia Story, The (1940)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>469</v>
+        <v>174</v>
       </c>
       <c r="B11" t="n">
-        <v>1249</v>
+        <v>1228</v>
       </c>
       <c r="C11" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D11" t="n">
-        <v>4.457306538071758</v>
+        <v>4.45816204340413</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Femme Nikita, La (Nikita) (1990)</t>
+          <t>Raging Bull (1980)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>235</v>
+        <v>174</v>
       </c>
       <c r="B12" t="n">
-        <v>1204</v>
+        <v>318</v>
       </c>
       <c r="C12" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D12" t="n">
-        <v>4.446471317185627</v>
+        <v>4.42859984738032</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Lawrence of Arabia (1962)</t>
+          <t>Shawshank Redemption, The (1994)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>235</v>
+        <v>174</v>
       </c>
       <c r="B13" t="n">
-        <v>50</v>
+        <v>1104</v>
       </c>
       <c r="C13" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D13" t="n">
-        <v>4.441849524979956</v>
+        <v>4.400974309271004</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Usual Suspects, The (1995)</t>
+          <t>Streetcar Named Desire, A (1951)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>235</v>
+        <v>174</v>
       </c>
       <c r="B14" t="n">
         <v>750</v>
@@ -699,7 +699,7 @@
         <v>3.579442714350294</v>
       </c>
       <c r="D14" t="n">
-        <v>4.440371228533754</v>
+        <v>4.389324783166678</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -709,134 +709,134 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B15" t="n">
-        <v>1208</v>
+        <v>246</v>
       </c>
       <c r="C15" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D15" t="n">
-        <v>4.425886316023822</v>
+        <v>3.678617047263723</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Apocalypse Now (1979)</t>
+          <t>Hoop Dreams (1994)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>334</v>
+        <v>230</v>
       </c>
       <c r="B16" t="n">
-        <v>1197</v>
+        <v>175</v>
       </c>
       <c r="C16" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D16" t="n">
-        <v>3.881221809677639</v>
+        <v>3.587518897839494</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Princess Bride, The (1987)</t>
+          <t>Kids (1995)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>334</v>
+        <v>230</v>
       </c>
       <c r="B17" t="n">
-        <v>1104</v>
+        <v>3683</v>
       </c>
       <c r="C17" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D17" t="n">
-        <v>3.809048463062753</v>
+        <v>3.576313211423831</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Streetcar Named Desire, A (1951)</t>
+          <t>Blood Simple (1984)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>334</v>
+        <v>230</v>
       </c>
       <c r="B18" t="n">
-        <v>912</v>
+        <v>53322</v>
       </c>
       <c r="C18" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D18" t="n">
-        <v>3.76591383523425</v>
+        <v>3.554824360513655</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Casablanca (1942)</t>
+          <t>Ocean's Thirteen (2007)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>334</v>
+        <v>230</v>
       </c>
       <c r="B19" t="n">
-        <v>1248</v>
+        <v>1298</v>
       </c>
       <c r="C19" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D19" t="n">
-        <v>3.747158294041225</v>
+        <v>3.485842551545808</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Touch of Evil (1958)</t>
+          <t>Pink Floyd: The Wall (1982)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>108</v>
+        <v>518</v>
       </c>
       <c r="B20" t="n">
-        <v>318</v>
+        <v>2360</v>
       </c>
       <c r="C20" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D20" t="n">
-        <v>4.819822135702879</v>
+        <v>4.499253831148236</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Shawshank Redemption, The (1994)</t>
+          <t>Celebration, The (Festen) (1998)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>108</v>
+        <v>518</v>
       </c>
       <c r="B21" t="n">
-        <v>904</v>
+        <v>177765</v>
       </c>
       <c r="C21" t="n">
         <v>3.579442714350294</v>
       </c>
       <c r="D21" t="n">
-        <v>4.689284119284837</v>
+        <v>4.447250796450595</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Rear Window (1954)</t>
+          <t>Coco (2017)</t>
         </is>
       </c>
     </row>

</xml_diff>